<commit_message>
added Qualification to profiles
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-NatlDirEndpointQry-Network.xlsx
+++ b/output/StructureDefinition-NatlDirEndpointQry-Network.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AM$74</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AM$75</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2632" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2667" uniqueCount="533">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-04-05T10:32:14-04:00</t>
+    <t>2022-04-05T18:50:47-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -620,6 +620,19 @@
   <si>
     <t xml:space="preserve">ele-1
 </t>
+  </si>
+  <si>
+    <t>qualification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://hl7.org/fhir/us/fhir-directory-query/StructureDefinition/qualification}
+</t>
+  </si>
+  <si>
+    <t>Qualification</t>
+  </si>
+  <si>
+    <t>An extension to add qualifications for an organization (e.g. accreditation) or practitionerRole (e.g. registered to prescribe controlled substances).</t>
   </si>
   <si>
     <t>Organization.modifierExtension</t>
@@ -1983,7 +1996,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AM74"/>
+  <dimension ref="A1:AM75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -4031,11 +4044,13 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="B19" t="s" s="2">
         <v>194</v>
       </c>
-      <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
-        <v>104</v>
+        <v>76</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
@@ -4048,26 +4063,22 @@
         <v>76</v>
       </c>
       <c r="H19" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="I19" t="s" s="2">
         <v>76</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>105</v>
+        <v>195</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>196</v>
-      </c>
-      <c r="M19" t="s" s="2">
-        <v>108</v>
-      </c>
-      <c r="N19" t="s" s="2">
         <v>197</v>
       </c>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
         <v>76</v>
       </c>
@@ -4115,7 +4126,7 @@
         <v>76</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>77</v>
@@ -4124,7 +4135,7 @@
         <v>78</v>
       </c>
       <c r="AH19" t="s" s="2">
-        <v>76</v>
+        <v>193</v>
       </c>
       <c r="AI19" t="s" s="2">
         <v>113</v>
@@ -4133,7 +4144,7 @@
         <v>76</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>184</v>
+        <v>76</v>
       </c>
       <c r="AL19" t="s" s="2">
         <v>76</v>
@@ -4144,11 +4155,11 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
@@ -4158,28 +4169,28 @@
         <v>78</v>
       </c>
       <c r="G20" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="H20" t="s" s="2">
         <v>86</v>
       </c>
-      <c r="H20" t="s" s="2">
-        <v>76</v>
-      </c>
       <c r="I20" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="J20" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="K20" t="s" s="2">
+        <v>199</v>
+      </c>
+      <c r="L20" t="s" s="2">
         <v>200</v>
       </c>
-      <c r="K20" t="s" s="2">
+      <c r="M20" t="s" s="2">
+        <v>108</v>
+      </c>
+      <c r="N20" t="s" s="2">
         <v>201</v>
-      </c>
-      <c r="L20" t="s" s="2">
-        <v>202</v>
-      </c>
-      <c r="M20" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="N20" t="s" s="2">
-        <v>204</v>
       </c>
       <c r="O20" t="s" s="2">
         <v>76</v>
@@ -4216,17 +4227,19 @@
         <v>76</v>
       </c>
       <c r="AA20" t="s" s="2">
-        <v>205</v>
-      </c>
-      <c r="AB20" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="AB20" t="s" s="2">
+        <v>76</v>
+      </c>
       <c r="AC20" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD20" t="s" s="2">
-        <v>111</v>
+        <v>76</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>77</v>
@@ -4235,27 +4248,27 @@
         <v>78</v>
       </c>
       <c r="AH20" t="s" s="2">
-        <v>206</v>
+        <v>76</v>
       </c>
       <c r="AI20" t="s" s="2">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>207</v>
+        <v>76</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>209</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -4266,28 +4279,32 @@
         <v>77</v>
       </c>
       <c r="F21" t="s" s="2">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="H21" t="s" s="2">
         <v>76</v>
       </c>
       <c r="I21" t="s" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>87</v>
+        <v>204</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>99</v>
+        <v>205</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>100</v>
-      </c>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
+        <v>206</v>
+      </c>
+      <c r="M21" t="s" s="2">
+        <v>207</v>
+      </c>
+      <c r="N21" t="s" s="2">
+        <v>208</v>
+      </c>
       <c r="O21" t="s" s="2">
         <v>76</v>
       </c>
@@ -4323,59 +4340,57 @@
         <v>76</v>
       </c>
       <c r="AA21" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB21" t="s" s="2">
-        <v>76</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="AB21" s="2"/>
       <c r="AC21" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD21" t="s" s="2">
-        <v>76</v>
+        <v>111</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>101</v>
+        <v>203</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG21" t="s" s="2">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="AH21" t="s" s="2">
-        <v>76</v>
+        <v>210</v>
       </c>
       <c r="AI21" t="s" s="2">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>76</v>
+        <v>211</v>
       </c>
       <c r="AK21" t="s" s="2">
+        <v>212</v>
+      </c>
+      <c r="AL21" t="s" s="2">
         <v>102</v>
       </c>
-      <c r="AL21" t="s" s="2">
-        <v>76</v>
-      </c>
       <c r="AM21" t="s" s="2">
-        <v>76</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
-        <v>104</v>
+        <v>76</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
         <v>77</v>
       </c>
       <c r="F22" t="s" s="2">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="G22" t="s" s="2">
         <v>76</v>
@@ -4387,17 +4402,15 @@
         <v>76</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>107</v>
-      </c>
-      <c r="M22" t="s" s="2">
-        <v>108</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" t="s" s="2">
         <v>76</v>
@@ -4434,31 +4447,31 @@
         <v>76</v>
       </c>
       <c r="AA22" t="s" s="2">
-        <v>109</v>
+        <v>76</v>
       </c>
       <c r="AB22" t="s" s="2">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="AC22" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD22" t="s" s="2">
-        <v>111</v>
+        <v>76</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG22" t="s" s="2">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="AH22" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI22" t="s" s="2">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="AJ22" t="s" s="2">
         <v>76</v>
@@ -4475,43 +4488,41 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
         <v>77</v>
       </c>
       <c r="F23" t="s" s="2">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>76</v>
       </c>
       <c r="H23" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="I23" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>161</v>
+        <v>105</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>213</v>
+        <v>106</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>214</v>
+        <v>107</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>215</v>
-      </c>
-      <c r="N23" t="s" s="2">
-        <v>216</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
         <v>76</v>
       </c>
@@ -4535,49 +4546,49 @@
         <v>76</v>
       </c>
       <c r="W23" t="s" s="2">
-        <v>217</v>
+        <v>76</v>
       </c>
       <c r="X23" t="s" s="2">
-        <v>218</v>
+        <v>76</v>
       </c>
       <c r="Y23" t="s" s="2">
-        <v>219</v>
+        <v>76</v>
       </c>
       <c r="Z23" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AA23" t="s" s="2">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="AB23" t="s" s="2">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="AC23" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD23" t="s" s="2">
-        <v>76</v>
+        <v>111</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>220</v>
+        <v>112</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG23" t="s" s="2">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="AH23" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>184</v>
+        <v>76</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>221</v>
+        <v>102</v>
       </c>
       <c r="AL23" t="s" s="2">
         <v>76</v>
@@ -4586,9 +4597,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4602,28 +4613,28 @@
         <v>85</v>
       </c>
       <c r="G24" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="H24" t="s" s="2">
         <v>86</v>
-      </c>
-      <c r="H24" t="s" s="2">
-        <v>76</v>
       </c>
       <c r="I24" t="s" s="2">
         <v>86</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>223</v>
+        <v>161</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>76</v>
@@ -4648,13 +4659,13 @@
         <v>76</v>
       </c>
       <c r="W24" t="s" s="2">
-        <v>143</v>
+        <v>221</v>
       </c>
       <c r="X24" t="s" s="2">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="Y24" t="s" s="2">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="Z24" t="s" s="2">
         <v>76</v>
@@ -4672,7 +4683,7 @@
         <v>76</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>77</v>
@@ -4687,10 +4698,10 @@
         <v>97</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="AL24" t="s" s="2">
         <v>76</v>
@@ -4701,7 +4712,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4724,19 +4735,19 @@
         <v>86</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>127</v>
+        <v>227</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>76</v>
@@ -4749,7 +4760,7 @@
         <v>76</v>
       </c>
       <c r="S25" t="s" s="2">
-        <v>237</v>
+        <v>76</v>
       </c>
       <c r="T25" t="s" s="2">
         <v>76</v>
@@ -4761,13 +4772,13 @@
         <v>76</v>
       </c>
       <c r="W25" t="s" s="2">
-        <v>76</v>
+        <v>143</v>
       </c>
       <c r="X25" t="s" s="2">
-        <v>76</v>
+        <v>232</v>
       </c>
       <c r="Y25" t="s" s="2">
-        <v>76</v>
+        <v>233</v>
       </c>
       <c r="Z25" t="s" s="2">
         <v>76</v>
@@ -4785,7 +4796,7 @@
         <v>76</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>77</v>
@@ -4800,13 +4811,13 @@
         <v>97</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>241</v>
+        <v>76</v>
       </c>
       <c r="AM25" t="s" s="2">
         <v>76</v>
@@ -4814,7 +4825,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4837,18 +4848,20 @@
         <v>86</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>87</v>
+        <v>127</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>245</v>
-      </c>
-      <c r="N26" s="2"/>
+        <v>239</v>
+      </c>
+      <c r="N26" t="s" s="2">
+        <v>240</v>
+      </c>
       <c r="O26" t="s" s="2">
         <v>76</v>
       </c>
@@ -4860,7 +4873,7 @@
         <v>76</v>
       </c>
       <c r="S26" t="s" s="2">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="T26" t="s" s="2">
         <v>76</v>
@@ -4896,7 +4909,7 @@
         <v>76</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>77</v>
@@ -4911,21 +4924,21 @@
         <v>97</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="AM26" t="s" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="27" hidden="true">
+    <row r="27">
       <c r="A27" t="s" s="2">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4939,7 +4952,7 @@
         <v>85</v>
       </c>
       <c r="G27" t="s" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="H27" t="s" s="2">
         <v>76</v>
@@ -4948,15 +4961,17 @@
         <v>86</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>252</v>
+        <v>87</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>254</v>
-      </c>
-      <c r="M27" s="2"/>
+        <v>248</v>
+      </c>
+      <c r="M27" t="s" s="2">
+        <v>249</v>
+      </c>
       <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
         <v>76</v>
@@ -4969,7 +4984,7 @@
         <v>76</v>
       </c>
       <c r="S27" t="s" s="2">
-        <v>76</v>
+        <v>250</v>
       </c>
       <c r="T27" t="s" s="2">
         <v>76</v>
@@ -5005,7 +5020,7 @@
         <v>76</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>77</v>
@@ -5020,21 +5035,21 @@
         <v>97</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="AM27" t="s" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -5048,7 +5063,7 @@
         <v>85</v>
       </c>
       <c r="G28" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="H28" t="s" s="2">
         <v>76</v>
@@ -5057,17 +5072,15 @@
         <v>86</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>262</v>
-      </c>
-      <c r="M28" t="s" s="2">
-        <v>263</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="M28" s="2"/>
       <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
         <v>76</v>
@@ -5116,7 +5129,7 @@
         <v>76</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>77</v>
@@ -5131,13 +5144,13 @@
         <v>97</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="AM28" t="s" s="2">
         <v>76</v>
@@ -5145,11 +5158,9 @@
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
-        <v>199</v>
-      </c>
-      <c r="B29" t="s" s="2">
-        <v>268</v>
-      </c>
+        <v>263</v>
+      </c>
+      <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
         <v>76</v>
       </c>
@@ -5170,18 +5181,18 @@
         <v>86</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>200</v>
+        <v>264</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>202</v>
-      </c>
-      <c r="M29" s="2"/>
-      <c r="N29" t="s" s="2">
-        <v>204</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="M29" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
         <v>76</v>
       </c>
@@ -5190,7 +5201,7 @@
         <v>76</v>
       </c>
       <c r="R29" t="s" s="2">
-        <v>270</v>
+        <v>76</v>
       </c>
       <c r="S29" t="s" s="2">
         <v>76</v>
@@ -5229,39 +5240,39 @@
         <v>76</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>199</v>
+        <v>268</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG29" t="s" s="2">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="AH29" t="s" s="2">
-        <v>206</v>
+        <v>76</v>
       </c>
       <c r="AI29" t="s" s="2">
         <v>97</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>207</v>
+        <v>269</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>208</v>
+        <v>270</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>102</v>
+        <v>271</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>209</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="30" hidden="true">
+    <row r="30">
       <c r="A30" t="s" s="2">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C30" t="s" s="2">
         <v>76</v>
@@ -5274,7 +5285,7 @@
         <v>85</v>
       </c>
       <c r="G30" t="s" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="H30" t="s" s="2">
         <v>76</v>
@@ -5283,17 +5294,17 @@
         <v>86</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="M30" s="2"/>
       <c r="N30" t="s" s="2">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="O30" t="s" s="2">
         <v>76</v>
@@ -5303,7 +5314,7 @@
         <v>76</v>
       </c>
       <c r="R30" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="S30" t="s" s="2">
         <v>76</v>
@@ -5342,7 +5353,7 @@
         <v>76</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>77</v>
@@ -5351,75 +5362,73 @@
         <v>78</v>
       </c>
       <c r="AH30" t="s" s="2">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="AI30" t="s" s="2">
         <v>97</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="AL30" t="s" s="2">
         <v>102</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>274</v>
-      </c>
-      <c r="B31" s="2"/>
+        <v>203</v>
+      </c>
+      <c r="B31" t="s" s="2">
+        <v>275</v>
+      </c>
       <c r="C31" t="s" s="2">
         <v>76</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F31" t="s" s="2">
         <v>85</v>
       </c>
       <c r="G31" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="H31" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="I31" t="s" s="2">
         <v>86</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>275</v>
+        <v>204</v>
       </c>
       <c r="K31" t="s" s="2">
         <v>276</v>
       </c>
       <c r="L31" t="s" s="2">
+        <v>206</v>
+      </c>
+      <c r="M31" s="2"/>
+      <c r="N31" t="s" s="2">
+        <v>208</v>
+      </c>
+      <c r="O31" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="P31" s="2"/>
+      <c r="Q31" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="R31" t="s" s="2">
         <v>277</v>
       </c>
-      <c r="M31" t="s" s="2">
-        <v>278</v>
-      </c>
-      <c r="N31" t="s" s="2">
-        <v>279</v>
-      </c>
-      <c r="O31" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="P31" t="s" s="2">
-        <v>280</v>
-      </c>
-      <c r="Q31" t="s" s="2">
-        <v>281</v>
-      </c>
-      <c r="R31" t="s" s="2">
-        <v>76</v>
-      </c>
       <c r="S31" t="s" s="2">
         <v>76</v>
       </c>
@@ -5457,36 +5466,36 @@
         <v>76</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG31" t="s" s="2">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="AH31" t="s" s="2">
-        <v>76</v>
+        <v>210</v>
       </c>
       <c r="AI31" t="s" s="2">
         <v>97</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>282</v>
+        <v>211</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>283</v>
+        <v>212</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>284</v>
+        <v>102</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>285</v>
+        <v>213</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5503,32 +5512,34 @@
         <v>86</v>
       </c>
       <c r="H32" t="s" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="I32" t="s" s="2">
         <v>86</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>223</v>
+        <v>279</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="N32" t="s" s="2">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="O32" t="s" s="2">
         <v>76</v>
       </c>
-      <c r="P32" s="2"/>
+      <c r="P32" t="s" s="2">
+        <v>284</v>
+      </c>
       <c r="Q32" t="s" s="2">
-        <v>76</v>
+        <v>285</v>
       </c>
       <c r="R32" t="s" s="2">
         <v>76</v>
@@ -5546,11 +5557,13 @@
         <v>76</v>
       </c>
       <c r="W32" t="s" s="2">
-        <v>217</v>
-      </c>
-      <c r="X32" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="X32" t="s" s="2">
+        <v>76</v>
+      </c>
       <c r="Y32" t="s" s="2">
-        <v>291</v>
+        <v>76</v>
       </c>
       <c r="Z32" t="s" s="2">
         <v>76</v>
@@ -5568,13 +5581,13 @@
         <v>76</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG32" t="s" s="2">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="AH32" t="s" s="2">
         <v>76</v>
@@ -5583,21 +5596,21 @@
         <v>97</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>102</v>
+        <v>288</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>294</v>
+        <v>289</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5620,19 +5633,19 @@
         <v>86</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>87</v>
+        <v>227</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="O33" t="s" s="2">
         <v>76</v>
@@ -5657,13 +5670,11 @@
         <v>76</v>
       </c>
       <c r="W33" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="X33" t="s" s="2">
-        <v>76</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="X33" s="2"/>
       <c r="Y33" t="s" s="2">
-        <v>76</v>
+        <v>295</v>
       </c>
       <c r="Z33" t="s" s="2">
         <v>76</v>
@@ -5681,36 +5692,36 @@
         <v>76</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG33" t="s" s="2">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="AH33" t="s" s="2">
-        <v>206</v>
+        <v>76</v>
       </c>
       <c r="AI33" t="s" s="2">
         <v>97</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>302</v>
+        <v>102</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>76</v>
+        <v>298</v>
       </c>
     </row>
-    <row r="34" hidden="true">
+    <row r="34">
       <c r="A34" t="s" s="2">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5718,34 +5729,34 @@
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="F34" t="s" s="2">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="G34" t="s" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="H34" t="s" s="2">
         <v>76</v>
       </c>
       <c r="I34" t="s" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="J34" t="s" s="2">
         <v>87</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="N34" t="s" s="2">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="O34" t="s" s="2">
         <v>76</v>
@@ -5794,36 +5805,36 @@
         <v>76</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG34" t="s" s="2">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="AH34" t="s" s="2">
-        <v>76</v>
+        <v>210</v>
       </c>
       <c r="AI34" t="s" s="2">
         <v>97</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>76</v>
+        <v>304</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>76</v>
+        <v>306</v>
       </c>
       <c r="AM34" t="s" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5834,10 +5845,10 @@
         <v>77</v>
       </c>
       <c r="F35" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G35" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="H35" t="s" s="2">
         <v>76</v>
@@ -5846,19 +5857,19 @@
         <v>76</v>
       </c>
       <c r="J35" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="K35" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="L35" t="s" s="2">
         <v>309</v>
       </c>
-      <c r="K35" t="s" s="2">
+      <c r="M35" t="s" s="2">
         <v>310</v>
       </c>
-      <c r="L35" t="s" s="2">
+      <c r="N35" t="s" s="2">
         <v>311</v>
-      </c>
-      <c r="M35" t="s" s="2">
-        <v>312</v>
-      </c>
-      <c r="N35" t="s" s="2">
-        <v>313</v>
       </c>
       <c r="O35" t="s" s="2">
         <v>76</v>
@@ -5907,7 +5918,7 @@
         <v>76</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>77</v>
@@ -5916,27 +5927,27 @@
         <v>78</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>314</v>
+        <v>76</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>315</v>
+        <v>97</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>316</v>
+        <v>76</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>317</v>
+        <v>305</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>318</v>
+        <v>76</v>
       </c>
       <c r="AM35" t="s" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="36" hidden="true">
+    <row r="36">
       <c r="A36" t="s" s="2">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5947,10 +5958,10 @@
         <v>77</v>
       </c>
       <c r="F36" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G36" t="s" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="H36" t="s" s="2">
         <v>76</v>
@@ -5959,16 +5970,20 @@
         <v>76</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>87</v>
+        <v>313</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>99</v>
+        <v>314</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>100</v>
-      </c>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
+        <v>315</v>
+      </c>
+      <c r="M36" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="N36" t="s" s="2">
+        <v>317</v>
+      </c>
       <c r="O36" t="s" s="2">
         <v>76</v>
       </c>
@@ -6016,28 +6031,28 @@
         <v>76</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>101</v>
+        <v>312</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG36" t="s" s="2">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>76</v>
+        <v>318</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>76</v>
+        <v>319</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>76</v>
+        <v>320</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>102</v>
+        <v>321</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>76</v>
+        <v>322</v>
       </c>
       <c r="AM36" t="s" s="2">
         <v>76</v>
@@ -6045,18 +6060,18 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
-        <v>104</v>
+        <v>76</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" t="s" s="2">
         <v>77</v>
       </c>
       <c r="F37" t="s" s="2">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="G37" t="s" s="2">
         <v>76</v>
@@ -6068,17 +6083,15 @@
         <v>76</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>107</v>
-      </c>
-      <c r="M37" t="s" s="2">
-        <v>108</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" t="s" s="2">
         <v>76</v>
@@ -6115,31 +6128,31 @@
         <v>76</v>
       </c>
       <c r="AA37" t="s" s="2">
-        <v>109</v>
+        <v>76</v>
       </c>
       <c r="AB37" t="s" s="2">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="AC37" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD37" t="s" s="2">
-        <v>111</v>
+        <v>76</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG37" t="s" s="2">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="AH37" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="AJ37" t="s" s="2">
         <v>76</v>
@@ -6154,40 +6167,42 @@
         <v>76</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" t="s" s="2">
         <v>77</v>
       </c>
       <c r="F38" t="s" s="2">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="H38" t="s" s="2">
         <v>76</v>
       </c>
       <c r="I38" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>161</v>
+        <v>105</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>322</v>
+        <v>106</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>323</v>
-      </c>
-      <c r="M38" s="2"/>
+        <v>107</v>
+      </c>
+      <c r="M38" t="s" s="2">
+        <v>108</v>
+      </c>
       <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
         <v>76</v>
@@ -6212,52 +6227,52 @@
         <v>76</v>
       </c>
       <c r="W38" t="s" s="2">
-        <v>217</v>
+        <v>76</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>324</v>
+        <v>76</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>325</v>
+        <v>76</v>
       </c>
       <c r="Z38" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AA38" t="s" s="2">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="AB38" t="s" s="2">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="AC38" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD38" t="s" s="2">
-        <v>76</v>
+        <v>111</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>326</v>
+        <v>112</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG38" t="s" s="2">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="AH38" t="s" s="2">
-        <v>327</v>
+        <v>76</v>
       </c>
       <c r="AI38" t="s" s="2">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>328</v>
+        <v>76</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>329</v>
+        <v>102</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>330</v>
+        <v>76</v>
       </c>
       <c r="AM38" t="s" s="2">
         <v>76</v>
@@ -6265,7 +6280,7 @@
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6288,20 +6303,16 @@
         <v>86</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>87</v>
+        <v>161</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>333</v>
-      </c>
-      <c r="M39" t="s" s="2">
-        <v>334</v>
-      </c>
-      <c r="N39" t="s" s="2">
-        <v>335</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
       <c r="O39" t="s" s="2">
         <v>76</v>
       </c>
@@ -6325,13 +6336,13 @@
         <v>76</v>
       </c>
       <c r="W39" t="s" s="2">
-        <v>76</v>
+        <v>221</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>76</v>
+        <v>328</v>
       </c>
       <c r="Y39" t="s" s="2">
-        <v>76</v>
+        <v>329</v>
       </c>
       <c r="Z39" t="s" s="2">
         <v>76</v>
@@ -6349,7 +6360,7 @@
         <v>76</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>77</v>
@@ -6358,27 +6369,27 @@
         <v>85</v>
       </c>
       <c r="AH39" t="s" s="2">
-        <v>76</v>
+        <v>331</v>
       </c>
       <c r="AI39" t="s" s="2">
         <v>97</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>250</v>
+        <v>334</v>
       </c>
       <c r="AM39" t="s" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="40" hidden="true">
+    <row r="40">
       <c r="A40" t="s" s="2">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6392,28 +6403,28 @@
         <v>85</v>
       </c>
       <c r="G40" t="s" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="H40" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="I40" t="s" s="2">
         <v>86</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>161</v>
+        <v>87</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>76</v>
@@ -6438,13 +6449,13 @@
         <v>76</v>
       </c>
       <c r="W40" t="s" s="2">
-        <v>217</v>
+        <v>76</v>
       </c>
       <c r="X40" t="s" s="2">
-        <v>344</v>
+        <v>76</v>
       </c>
       <c r="Y40" t="s" s="2">
-        <v>345</v>
+        <v>76</v>
       </c>
       <c r="Z40" t="s" s="2">
         <v>76</v>
@@ -6462,7 +6473,7 @@
         <v>76</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>77</v>
@@ -6477,13 +6488,13 @@
         <v>97</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>349</v>
+        <v>254</v>
       </c>
       <c r="AM40" t="s" s="2">
         <v>76</v>
@@ -6491,7 +6502,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6508,24 +6519,26 @@
         <v>76</v>
       </c>
       <c r="H41" t="s" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="I41" t="s" s="2">
         <v>86</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>351</v>
+        <v>161</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>354</v>
-      </c>
-      <c r="N41" s="2"/>
+        <v>346</v>
+      </c>
+      <c r="N41" t="s" s="2">
+        <v>347</v>
+      </c>
       <c r="O41" t="s" s="2">
         <v>76</v>
       </c>
@@ -6549,13 +6562,13 @@
         <v>76</v>
       </c>
       <c r="W41" t="s" s="2">
-        <v>76</v>
+        <v>221</v>
       </c>
       <c r="X41" t="s" s="2">
-        <v>76</v>
+        <v>348</v>
       </c>
       <c r="Y41" t="s" s="2">
-        <v>76</v>
+        <v>349</v>
       </c>
       <c r="Z41" t="s" s="2">
         <v>76</v>
@@ -6573,7 +6586,7 @@
         <v>76</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>77</v>
@@ -6588,13 +6601,13 @@
         <v>97</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>102</v>
+        <v>351</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>102</v>
+        <v>352</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>76</v>
+        <v>353</v>
       </c>
       <c r="AM41" t="s" s="2">
         <v>76</v>
@@ -6602,7 +6615,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6625,15 +6638,17 @@
         <v>86</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>252</v>
+        <v>355</v>
       </c>
       <c r="K42" t="s" s="2">
+        <v>356</v>
+      </c>
+      <c r="L42" t="s" s="2">
         <v>357</v>
       </c>
-      <c r="L42" t="s" s="2">
+      <c r="M42" t="s" s="2">
         <v>358</v>
       </c>
-      <c r="M42" s="2"/>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
         <v>76</v>
@@ -6697,21 +6712,21 @@
         <v>97</v>
       </c>
       <c r="AJ42" t="s" s="2">
-        <v>184</v>
+        <v>102</v>
       </c>
       <c r="AK42" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="AL42" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AM42" t="s" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" hidden="true">
+      <c r="A43" t="s" s="2">
         <v>360</v>
-      </c>
-      <c r="AL42" t="s" s="2">
-        <v>258</v>
-      </c>
-      <c r="AM42" t="s" s="2">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="s" s="2">
-        <v>361</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6725,29 +6740,25 @@
         <v>85</v>
       </c>
       <c r="G43" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="H43" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="I43" t="s" s="2">
         <v>86</v>
       </c>
-      <c r="H43" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="I43" t="s" s="2">
-        <v>76</v>
-      </c>
       <c r="J43" t="s" s="2">
+        <v>256</v>
+      </c>
+      <c r="K43" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="L43" t="s" s="2">
         <v>362</v>
       </c>
-      <c r="K43" t="s" s="2">
-        <v>363</v>
-      </c>
-      <c r="L43" t="s" s="2">
-        <v>364</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>365</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>366</v>
-      </c>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
         <v>76</v>
       </c>
@@ -6795,36 +6806,36 @@
         <v>76</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG43" t="s" s="2">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="AH43" t="s" s="2">
-        <v>367</v>
+        <v>76</v>
       </c>
       <c r="AI43" t="s" s="2">
-        <v>368</v>
+        <v>97</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>369</v>
+        <v>184</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>102</v>
+        <v>262</v>
       </c>
       <c r="AM43" t="s" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="44" hidden="true">
+    <row r="44">
       <c r="A44" t="s" s="2">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6838,7 +6849,7 @@
         <v>85</v>
       </c>
       <c r="G44" t="s" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="H44" t="s" s="2">
         <v>76</v>
@@ -6847,16 +6858,20 @@
         <v>76</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>87</v>
+        <v>366</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>99</v>
+        <v>367</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>100</v>
-      </c>
-      <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
+        <v>368</v>
+      </c>
+      <c r="M44" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="N44" t="s" s="2">
+        <v>370</v>
+      </c>
       <c r="O44" t="s" s="2">
         <v>76</v>
       </c>
@@ -6904,28 +6919,28 @@
         <v>76</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>101</v>
+        <v>365</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG44" t="s" s="2">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="AH44" t="s" s="2">
-        <v>76</v>
+        <v>371</v>
       </c>
       <c r="AI44" t="s" s="2">
-        <v>76</v>
+        <v>372</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>76</v>
+        <v>373</v>
       </c>
       <c r="AK44" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="AL44" t="s" s="2">
         <v>102</v>
-      </c>
-      <c r="AL44" t="s" s="2">
-        <v>76</v>
       </c>
       <c r="AM44" t="s" s="2">
         <v>76</v>
@@ -6933,18 +6948,18 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
-        <v>104</v>
+        <v>76</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" t="s" s="2">
         <v>77</v>
       </c>
       <c r="F45" t="s" s="2">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="G45" t="s" s="2">
         <v>76</v>
@@ -6956,17 +6971,15 @@
         <v>76</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>107</v>
-      </c>
-      <c r="M45" t="s" s="2">
-        <v>108</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="M45" s="2"/>
       <c r="N45" s="2"/>
       <c r="O45" t="s" s="2">
         <v>76</v>
@@ -7003,31 +7016,31 @@
         <v>76</v>
       </c>
       <c r="AA45" t="s" s="2">
-        <v>109</v>
+        <v>76</v>
       </c>
       <c r="AB45" t="s" s="2">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="AC45" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD45" t="s" s="2">
-        <v>111</v>
+        <v>76</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG45" t="s" s="2">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="AH45" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="AJ45" t="s" s="2">
         <v>76</v>
@@ -7044,43 +7057,41 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" t="s" s="2">
         <v>77</v>
       </c>
       <c r="F46" t="s" s="2">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="G46" t="s" s="2">
         <v>76</v>
       </c>
       <c r="H46" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="I46" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>161</v>
+        <v>105</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>374</v>
+        <v>106</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>375</v>
+        <v>107</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>376</v>
-      </c>
-      <c r="N46" t="s" s="2">
-        <v>377</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
         <v>76</v>
       </c>
@@ -7092,7 +7103,7 @@
         <v>76</v>
       </c>
       <c r="S46" t="s" s="2">
-        <v>378</v>
+        <v>76</v>
       </c>
       <c r="T46" t="s" s="2">
         <v>76</v>
@@ -7104,52 +7115,52 @@
         <v>76</v>
       </c>
       <c r="W46" t="s" s="2">
-        <v>217</v>
+        <v>76</v>
       </c>
       <c r="X46" t="s" s="2">
-        <v>379</v>
+        <v>76</v>
       </c>
       <c r="Y46" t="s" s="2">
-        <v>380</v>
+        <v>76</v>
       </c>
       <c r="Z46" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AA46" t="s" s="2">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="AB46" t="s" s="2">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="AC46" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD46" t="s" s="2">
-        <v>76</v>
+        <v>111</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>381</v>
+        <v>112</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG46" t="s" s="2">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="AH46" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI46" t="s" s="2">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>382</v>
+        <v>76</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>348</v>
+        <v>102</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>383</v>
+        <v>76</v>
       </c>
       <c r="AM46" t="s" s="2">
         <v>76</v>
@@ -7157,7 +7168,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -7174,7 +7185,7 @@
         <v>76</v>
       </c>
       <c r="H47" t="s" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="I47" t="s" s="2">
         <v>86</v>
@@ -7183,15 +7194,17 @@
         <v>161</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>387</v>
-      </c>
-      <c r="N47" s="2"/>
+        <v>380</v>
+      </c>
+      <c r="N47" t="s" s="2">
+        <v>381</v>
+      </c>
       <c r="O47" t="s" s="2">
         <v>76</v>
       </c>
@@ -7203,7 +7216,7 @@
         <v>76</v>
       </c>
       <c r="S47" t="s" s="2">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="T47" t="s" s="2">
         <v>76</v>
@@ -7215,13 +7228,13 @@
         <v>76</v>
       </c>
       <c r="W47" t="s" s="2">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="X47" t="s" s="2">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="Y47" t="s" s="2">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="Z47" t="s" s="2">
         <v>76</v>
@@ -7239,7 +7252,7 @@
         <v>76</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>77</v>
@@ -7254,13 +7267,13 @@
         <v>97</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>76</v>
+        <v>387</v>
       </c>
       <c r="AM47" t="s" s="2">
         <v>76</v>
@@ -7268,7 +7281,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -7291,20 +7304,18 @@
         <v>86</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>87</v>
+        <v>161</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>396</v>
-      </c>
-      <c r="N48" t="s" s="2">
-        <v>397</v>
-      </c>
+        <v>391</v>
+      </c>
+      <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
         <v>76</v>
       </c>
@@ -7316,7 +7327,7 @@
         <v>76</v>
       </c>
       <c r="S48" t="s" s="2">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="T48" t="s" s="2">
         <v>76</v>
@@ -7328,13 +7339,13 @@
         <v>76</v>
       </c>
       <c r="W48" t="s" s="2">
-        <v>76</v>
+        <v>221</v>
       </c>
       <c r="X48" t="s" s="2">
-        <v>76</v>
+        <v>393</v>
       </c>
       <c r="Y48" t="s" s="2">
-        <v>76</v>
+        <v>394</v>
       </c>
       <c r="Z48" t="s" s="2">
         <v>76</v>
@@ -7352,7 +7363,7 @@
         <v>76</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>77</v>
@@ -7367,10 +7378,10 @@
         <v>97</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>401</v>
+        <v>352</v>
       </c>
       <c r="AL48" t="s" s="2">
         <v>76</v>
@@ -7379,9 +7390,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7392,10 +7403,10 @@
         <v>77</v>
       </c>
       <c r="F49" t="s" s="2">
-        <v>403</v>
+        <v>85</v>
       </c>
       <c r="G49" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="H49" t="s" s="2">
         <v>76</v>
@@ -7407,13 +7418,17 @@
         <v>87</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>405</v>
-      </c>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
+        <v>399</v>
+      </c>
+      <c r="M49" t="s" s="2">
+        <v>400</v>
+      </c>
+      <c r="N49" t="s" s="2">
+        <v>401</v>
+      </c>
       <c r="O49" t="s" s="2">
         <v>76</v>
       </c>
@@ -7425,7 +7440,7 @@
         <v>76</v>
       </c>
       <c r="S49" t="s" s="2">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="T49" t="s" s="2">
         <v>76</v>
@@ -7461,13 +7476,13 @@
         <v>76</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG49" t="s" s="2">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="AH49" t="s" s="2">
         <v>76</v>
@@ -7476,13 +7491,13 @@
         <v>97</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>410</v>
+        <v>76</v>
       </c>
       <c r="AM49" t="s" s="2">
         <v>76</v>
@@ -7490,18 +7505,18 @@
     </row>
     <row r="50">
       <c r="A50" t="s" s="2">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
-        <v>412</v>
+        <v>76</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
         <v>77</v>
       </c>
       <c r="F50" t="s" s="2">
-        <v>85</v>
+        <v>407</v>
       </c>
       <c r="G50" t="s" s="2">
         <v>86</v>
@@ -7516,10 +7531,10 @@
         <v>87</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -7534,7 +7549,7 @@
         <v>76</v>
       </c>
       <c r="S50" t="s" s="2">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="T50" t="s" s="2">
         <v>76</v>
@@ -7570,13 +7585,13 @@
         <v>76</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG50" t="s" s="2">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="AH50" t="s" s="2">
         <v>76</v>
@@ -7585,25 +7600,25 @@
         <v>97</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="AM50" t="s" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="51" hidden="true">
+    <row r="51">
       <c r="A51" t="s" s="2">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" t="s" s="2">
@@ -7613,7 +7628,7 @@
         <v>85</v>
       </c>
       <c r="G51" t="s" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="H51" t="s" s="2">
         <v>76</v>
@@ -7625,14 +7640,12 @@
         <v>87</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>423</v>
-      </c>
-      <c r="M51" t="s" s="2">
-        <v>424</v>
-      </c>
+        <v>418</v>
+      </c>
+      <c r="M51" s="2"/>
       <c r="N51" s="2"/>
       <c r="O51" t="s" s="2">
         <v>76</v>
@@ -7645,7 +7658,7 @@
         <v>76</v>
       </c>
       <c r="S51" t="s" s="2">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="T51" t="s" s="2">
         <v>76</v>
@@ -7681,7 +7694,7 @@
         <v>76</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>77</v>
@@ -7696,25 +7709,25 @@
         <v>97</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>76</v>
+        <v>423</v>
       </c>
       <c r="AM51" t="s" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" t="s" s="2">
@@ -7724,7 +7737,7 @@
         <v>85</v>
       </c>
       <c r="G52" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="H52" t="s" s="2">
         <v>76</v>
@@ -7736,12 +7749,14 @@
         <v>87</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>432</v>
-      </c>
-      <c r="M52" s="2"/>
+        <v>427</v>
+      </c>
+      <c r="M52" t="s" s="2">
+        <v>428</v>
+      </c>
       <c r="N52" s="2"/>
       <c r="O52" t="s" s="2">
         <v>76</v>
@@ -7754,7 +7769,7 @@
         <v>76</v>
       </c>
       <c r="S52" t="s" s="2">
-        <v>76</v>
+        <v>429</v>
       </c>
       <c r="T52" t="s" s="2">
         <v>76</v>
@@ -7766,13 +7781,13 @@
         <v>76</v>
       </c>
       <c r="W52" t="s" s="2">
-        <v>143</v>
+        <v>76</v>
       </c>
       <c r="X52" t="s" s="2">
-        <v>433</v>
+        <v>76</v>
       </c>
       <c r="Y52" t="s" s="2">
-        <v>434</v>
+        <v>76</v>
       </c>
       <c r="Z52" t="s" s="2">
         <v>76</v>
@@ -7790,7 +7805,7 @@
         <v>76</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>77</v>
@@ -7805,13 +7820,13 @@
         <v>97</v>
       </c>
       <c r="AJ52" t="s" s="2">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>438</v>
+        <v>76</v>
       </c>
       <c r="AM52" t="s" s="2">
         <v>76</v>
@@ -7819,11 +7834,11 @@
     </row>
     <row r="53">
       <c r="A53" t="s" s="2">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" t="s" s="2">
@@ -7845,10 +7860,10 @@
         <v>87</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -7863,7 +7878,7 @@
         <v>76</v>
       </c>
       <c r="S53" t="s" s="2">
-        <v>443</v>
+        <v>76</v>
       </c>
       <c r="T53" t="s" s="2">
         <v>76</v>
@@ -7875,13 +7890,13 @@
         <v>76</v>
       </c>
       <c r="W53" t="s" s="2">
-        <v>76</v>
+        <v>143</v>
       </c>
       <c r="X53" t="s" s="2">
-        <v>76</v>
+        <v>437</v>
       </c>
       <c r="Y53" t="s" s="2">
-        <v>76</v>
+        <v>438</v>
       </c>
       <c r="Z53" t="s" s="2">
         <v>76</v>
@@ -7899,7 +7914,7 @@
         <v>76</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>77</v>
@@ -7914,13 +7929,13 @@
         <v>97</v>
       </c>
       <c r="AJ53" t="s" s="2">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="AM53" t="s" s="2">
         <v>76</v>
@@ -7928,11 +7943,11 @@
     </row>
     <row r="54">
       <c r="A54" t="s" s="2">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
-        <v>76</v>
+        <v>444</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" t="s" s="2">
@@ -7954,14 +7969,12 @@
         <v>87</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>450</v>
-      </c>
-      <c r="M54" t="s" s="2">
-        <v>451</v>
-      </c>
+        <v>446</v>
+      </c>
+      <c r="M54" s="2"/>
       <c r="N54" s="2"/>
       <c r="O54" t="s" s="2">
         <v>76</v>
@@ -7974,7 +7987,7 @@
         <v>76</v>
       </c>
       <c r="S54" t="s" s="2">
-        <v>76</v>
+        <v>447</v>
       </c>
       <c r="T54" t="s" s="2">
         <v>76</v>
@@ -8010,7 +8023,7 @@
         <v>76</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>77</v>
@@ -8025,21 +8038,21 @@
         <v>97</v>
       </c>
       <c r="AJ54" t="s" s="2">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="AM54" t="s" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="55" hidden="true">
+    <row r="55">
       <c r="A55" t="s" s="2">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -8053,7 +8066,7 @@
         <v>85</v>
       </c>
       <c r="G55" t="s" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="H55" t="s" s="2">
         <v>76</v>
@@ -8062,18 +8075,18 @@
         <v>86</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>252</v>
+        <v>87</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>458</v>
-      </c>
-      <c r="M55" s="2"/>
-      <c r="N55" t="s" s="2">
-        <v>459</v>
-      </c>
+        <v>454</v>
+      </c>
+      <c r="M55" t="s" s="2">
+        <v>455</v>
+      </c>
+      <c r="N55" s="2"/>
       <c r="O55" t="s" s="2">
         <v>76</v>
       </c>
@@ -8085,7 +8098,7 @@
         <v>76</v>
       </c>
       <c r="S55" t="s" s="2">
-        <v>460</v>
+        <v>76</v>
       </c>
       <c r="T55" t="s" s="2">
         <v>76</v>
@@ -8121,7 +8134,7 @@
         <v>76</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>77</v>
@@ -8136,21 +8149,21 @@
         <v>97</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>360</v>
+        <v>458</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>258</v>
+        <v>459</v>
       </c>
       <c r="AM55" t="s" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -8158,13 +8171,13 @@
       </c>
       <c r="D56" s="2"/>
       <c r="E56" t="s" s="2">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F56" t="s" s="2">
         <v>85</v>
       </c>
       <c r="G56" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="H56" t="s" s="2">
         <v>76</v>
@@ -8173,17 +8186,17 @@
         <v>86</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>464</v>
+        <v>256</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="M56" s="2"/>
       <c r="N56" t="s" s="2">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="O56" t="s" s="2">
         <v>76</v>
@@ -8196,7 +8209,7 @@
         <v>76</v>
       </c>
       <c r="S56" t="s" s="2">
-        <v>76</v>
+        <v>464</v>
       </c>
       <c r="T56" t="s" s="2">
         <v>76</v>
@@ -8232,7 +8245,7 @@
         <v>76</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>77</v>
@@ -8247,13 +8260,13 @@
         <v>97</v>
       </c>
       <c r="AJ56" t="s" s="2">
-        <v>282</v>
+        <v>466</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>468</v>
+        <v>364</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>102</v>
+        <v>262</v>
       </c>
       <c r="AM56" t="s" s="2">
         <v>76</v>
@@ -8261,7 +8274,7 @@
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -8269,10 +8282,10 @@
       </c>
       <c r="D57" s="2"/>
       <c r="E57" t="s" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="F57" t="s" s="2">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="G57" t="s" s="2">
         <v>86</v>
@@ -8281,22 +8294,20 @@
         <v>76</v>
       </c>
       <c r="I57" t="s" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="J57" t="s" s="2">
+        <v>468</v>
+      </c>
+      <c r="K57" t="s" s="2">
+        <v>469</v>
+      </c>
+      <c r="L57" t="s" s="2">
         <v>470</v>
       </c>
-      <c r="K57" t="s" s="2">
+      <c r="M57" s="2"/>
+      <c r="N57" t="s" s="2">
         <v>471</v>
-      </c>
-      <c r="L57" t="s" s="2">
-        <v>472</v>
-      </c>
-      <c r="M57" t="s" s="2">
-        <v>473</v>
-      </c>
-      <c r="N57" t="s" s="2">
-        <v>474</v>
       </c>
       <c r="O57" t="s" s="2">
         <v>76</v>
@@ -8345,13 +8356,13 @@
         <v>76</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG57" t="s" s="2">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="AH57" t="s" s="2">
         <v>76</v>
@@ -8360,21 +8371,21 @@
         <v>97</v>
       </c>
       <c r="AJ57" t="s" s="2">
-        <v>76</v>
+        <v>286</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="AM57" t="s" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="58" hidden="true">
+    <row r="58">
       <c r="A58" t="s" s="2">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -8385,10 +8396,10 @@
         <v>77</v>
       </c>
       <c r="F58" t="s" s="2">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="G58" t="s" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="H58" t="s" s="2">
         <v>76</v>
@@ -8397,16 +8408,20 @@
         <v>76</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>87</v>
+        <v>474</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>99</v>
+        <v>475</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>100</v>
-      </c>
-      <c r="M58" s="2"/>
-      <c r="N58" s="2"/>
+        <v>476</v>
+      </c>
+      <c r="M58" t="s" s="2">
+        <v>477</v>
+      </c>
+      <c r="N58" t="s" s="2">
+        <v>478</v>
+      </c>
       <c r="O58" t="s" s="2">
         <v>76</v>
       </c>
@@ -8454,25 +8469,25 @@
         <v>76</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>101</v>
+        <v>473</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG58" t="s" s="2">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="AH58" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI58" t="s" s="2">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="AJ58" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>102</v>
+        <v>479</v>
       </c>
       <c r="AL58" t="s" s="2">
         <v>76</v>
@@ -8483,18 +8498,18 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
-        <v>104</v>
+        <v>76</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" t="s" s="2">
         <v>77</v>
       </c>
       <c r="F59" t="s" s="2">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="G59" t="s" s="2">
         <v>76</v>
@@ -8506,17 +8521,15 @@
         <v>76</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>107</v>
-      </c>
-      <c r="M59" t="s" s="2">
-        <v>108</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="M59" s="2"/>
       <c r="N59" s="2"/>
       <c r="O59" t="s" s="2">
         <v>76</v>
@@ -8565,19 +8578,19 @@
         <v>76</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG59" t="s" s="2">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="AH59" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI59" t="s" s="2">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="AJ59" t="s" s="2">
         <v>76</v>
@@ -8594,11 +8607,11 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
-        <v>479</v>
+        <v>104</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" t="s" s="2">
@@ -8611,26 +8624,24 @@
         <v>76</v>
       </c>
       <c r="H60" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="I60" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="J60" t="s" s="2">
         <v>105</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>480</v>
+        <v>106</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>481</v>
+        <v>107</v>
       </c>
       <c r="M60" t="s" s="2">
         <v>108</v>
       </c>
-      <c r="N60" t="s" s="2">
-        <v>197</v>
-      </c>
+      <c r="N60" s="2"/>
       <c r="O60" t="s" s="2">
         <v>76</v>
       </c>
@@ -8678,7 +8689,7 @@
         <v>76</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>482</v>
+        <v>112</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>77</v>
@@ -8696,7 +8707,7 @@
         <v>76</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>184</v>
+        <v>102</v>
       </c>
       <c r="AL60" t="s" s="2">
         <v>76</v>
@@ -8707,30 +8718,30 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
-        <v>76</v>
+        <v>483</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" t="s" s="2">
         <v>77</v>
       </c>
       <c r="F61" t="s" s="2">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="G61" t="s" s="2">
         <v>76</v>
       </c>
       <c r="H61" t="s" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="I61" t="s" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>223</v>
+        <v>105</v>
       </c>
       <c r="K61" t="s" s="2">
         <v>484</v>
@@ -8738,9 +8749,11 @@
       <c r="L61" t="s" s="2">
         <v>485</v>
       </c>
-      <c r="M61" s="2"/>
+      <c r="M61" t="s" s="2">
+        <v>108</v>
+      </c>
       <c r="N61" t="s" s="2">
-        <v>486</v>
+        <v>201</v>
       </c>
       <c r="O61" t="s" s="2">
         <v>76</v>
@@ -8765,60 +8778,60 @@
         <v>76</v>
       </c>
       <c r="W61" t="s" s="2">
-        <v>143</v>
+        <v>76</v>
       </c>
       <c r="X61" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="Y61" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="Z61" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AA61" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AB61" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AC61" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AD61" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE61" t="s" s="2">
+        <v>486</v>
+      </c>
+      <c r="AF61" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AG61" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH61" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AI61" t="s" s="2">
+        <v>113</v>
+      </c>
+      <c r="AJ61" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AK61" t="s" s="2">
+        <v>184</v>
+      </c>
+      <c r="AL61" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AM61" t="s" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="62" hidden="true">
+      <c r="A62" t="s" s="2">
         <v>487</v>
-      </c>
-      <c r="Y61" t="s" s="2">
-        <v>488</v>
-      </c>
-      <c r="Z61" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AA61" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB61" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AC61" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AD61" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE61" t="s" s="2">
-        <v>483</v>
-      </c>
-      <c r="AF61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AG61" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="AH61" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AI61" t="s" s="2">
-        <v>97</v>
-      </c>
-      <c r="AJ61" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AK61" t="s" s="2">
-        <v>489</v>
-      </c>
-      <c r="AL61" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AM61" t="s" s="2">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="s" s="2">
-        <v>490</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8832,7 +8845,7 @@
         <v>85</v>
       </c>
       <c r="G62" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="H62" t="s" s="2">
         <v>76</v>
@@ -8841,17 +8854,17 @@
         <v>76</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>491</v>
+        <v>227</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="M62" s="2"/>
       <c r="N62" t="s" s="2">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="O62" t="s" s="2">
         <v>76</v>
@@ -8876,13 +8889,13 @@
         <v>76</v>
       </c>
       <c r="W62" t="s" s="2">
-        <v>76</v>
+        <v>143</v>
       </c>
       <c r="X62" t="s" s="2">
-        <v>76</v>
+        <v>491</v>
       </c>
       <c r="Y62" t="s" s="2">
-        <v>76</v>
+        <v>492</v>
       </c>
       <c r="Z62" t="s" s="2">
         <v>76</v>
@@ -8900,7 +8913,7 @@
         <v>76</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>77</v>
@@ -8915,10 +8928,10 @@
         <v>97</v>
       </c>
       <c r="AJ62" t="s" s="2">
-        <v>495</v>
+        <v>76</v>
       </c>
       <c r="AK62" t="s" s="2">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="AL62" t="s" s="2">
         <v>76</v>
@@ -8929,7 +8942,7 @@
     </row>
     <row r="63">
       <c r="A63" t="s" s="2">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8940,7 +8953,7 @@
         <v>77</v>
       </c>
       <c r="F63" t="s" s="2">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="G63" t="s" s="2">
         <v>86</v>
@@ -8952,17 +8965,17 @@
         <v>76</v>
       </c>
       <c r="J63" t="s" s="2">
-        <v>309</v>
+        <v>495</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="M63" s="2"/>
       <c r="N63" t="s" s="2">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="O63" t="s" s="2">
         <v>76</v>
@@ -9011,13 +9024,13 @@
         <v>76</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG63" t="s" s="2">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="AH63" t="s" s="2">
         <v>76</v>
@@ -9026,21 +9039,21 @@
         <v>97</v>
       </c>
       <c r="AJ63" t="s" s="2">
+        <v>499</v>
+      </c>
+      <c r="AK63" t="s" s="2">
+        <v>500</v>
+      </c>
+      <c r="AL63" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AM63" t="s" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s" s="2">
         <v>501</v>
-      </c>
-      <c r="AK63" t="s" s="2">
-        <v>502</v>
-      </c>
-      <c r="AL63" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AM63" t="s" s="2">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="64" hidden="true">
-      <c r="A64" t="s" s="2">
-        <v>503</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -9051,10 +9064,10 @@
         <v>77</v>
       </c>
       <c r="F64" t="s" s="2">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="G64" t="s" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="H64" t="s" s="2">
         <v>76</v>
@@ -9063,16 +9076,18 @@
         <v>76</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>87</v>
+        <v>313</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>99</v>
+        <v>502</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>100</v>
+        <v>503</v>
       </c>
       <c r="M64" s="2"/>
-      <c r="N64" s="2"/>
+      <c r="N64" t="s" s="2">
+        <v>504</v>
+      </c>
       <c r="O64" t="s" s="2">
         <v>76</v>
       </c>
@@ -9120,25 +9135,25 @@
         <v>76</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>101</v>
+        <v>501</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG64" t="s" s="2">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="AH64" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI64" t="s" s="2">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="AJ64" t="s" s="2">
-        <v>76</v>
+        <v>505</v>
       </c>
       <c r="AK64" t="s" s="2">
-        <v>102</v>
+        <v>506</v>
       </c>
       <c r="AL64" t="s" s="2">
         <v>76</v>
@@ -9149,18 +9164,18 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
-        <v>104</v>
+        <v>76</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" t="s" s="2">
         <v>77</v>
       </c>
       <c r="F65" t="s" s="2">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="G65" t="s" s="2">
         <v>76</v>
@@ -9172,17 +9187,15 @@
         <v>76</v>
       </c>
       <c r="J65" t="s" s="2">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>107</v>
-      </c>
-      <c r="M65" t="s" s="2">
-        <v>108</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="M65" s="2"/>
       <c r="N65" s="2"/>
       <c r="O65" t="s" s="2">
         <v>76</v>
@@ -9219,31 +9232,31 @@
         <v>76</v>
       </c>
       <c r="AA65" t="s" s="2">
-        <v>109</v>
+        <v>76</v>
       </c>
       <c r="AB65" t="s" s="2">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="AC65" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD65" t="s" s="2">
-        <v>111</v>
+        <v>76</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG65" t="s" s="2">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="AH65" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AI65" t="s" s="2">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="AJ65" t="s" s="2">
         <v>76</v>
@@ -9260,13 +9273,11 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>504</v>
-      </c>
-      <c r="B66" t="s" s="2">
-        <v>505</v>
-      </c>
+        <v>508</v>
+      </c>
+      <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" t="s" s="2">
@@ -9285,15 +9296,17 @@
         <v>76</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>506</v>
+        <v>105</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>507</v>
+        <v>106</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>508</v>
-      </c>
-      <c r="M66" s="2"/>
+        <v>107</v>
+      </c>
+      <c r="M66" t="s" s="2">
+        <v>108</v>
+      </c>
       <c r="N66" s="2"/>
       <c r="O66" t="s" s="2">
         <v>76</v>
@@ -9330,16 +9343,16 @@
         <v>76</v>
       </c>
       <c r="AA66" t="s" s="2">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="AB66" t="s" s="2">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="AC66" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AD66" t="s" s="2">
-        <v>76</v>
+        <v>111</v>
       </c>
       <c r="AE66" t="s" s="2">
         <v>112</v>
@@ -9360,7 +9373,7 @@
         <v>76</v>
       </c>
       <c r="AK66" t="s" s="2">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="AL66" t="s" s="2">
         <v>76</v>
@@ -9371,7 +9384,7 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="B67" t="s" s="2">
         <v>509</v>
@@ -9480,11 +9493,13 @@
         <v>76</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
+        <v>508</v>
+      </c>
+      <c r="B68" t="s" s="2">
         <v>513</v>
       </c>
-      <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
         <v>76</v>
       </c>
@@ -9493,25 +9508,25 @@
         <v>77</v>
       </c>
       <c r="F68" t="s" s="2">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="G68" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="H68" t="s" s="2">
         <v>76</v>
       </c>
       <c r="I68" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="J68" t="s" s="2">
-        <v>161</v>
+        <v>514</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>322</v>
+        <v>515</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>323</v>
+        <v>516</v>
       </c>
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
@@ -9538,13 +9553,13 @@
         <v>76</v>
       </c>
       <c r="W68" t="s" s="2">
-        <v>217</v>
+        <v>76</v>
       </c>
       <c r="X68" t="s" s="2">
-        <v>324</v>
+        <v>76</v>
       </c>
       <c r="Y68" t="s" s="2">
-        <v>325</v>
+        <v>76</v>
       </c>
       <c r="Z68" t="s" s="2">
         <v>76</v>
@@ -9562,28 +9577,28 @@
         <v>76</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>326</v>
+        <v>112</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG68" t="s" s="2">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="AH68" t="s" s="2">
-        <v>327</v>
+        <v>76</v>
       </c>
       <c r="AI68" t="s" s="2">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="AJ68" t="s" s="2">
-        <v>328</v>
+        <v>76</v>
       </c>
       <c r="AK68" t="s" s="2">
-        <v>329</v>
+        <v>76</v>
       </c>
       <c r="AL68" t="s" s="2">
-        <v>330</v>
+        <v>76</v>
       </c>
       <c r="AM68" t="s" s="2">
         <v>76</v>
@@ -9591,7 +9606,7 @@
     </row>
     <row r="69">
       <c r="A69" t="s" s="2">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -9614,20 +9629,16 @@
         <v>86</v>
       </c>
       <c r="J69" t="s" s="2">
-        <v>87</v>
+        <v>161</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>333</v>
-      </c>
-      <c r="M69" t="s" s="2">
-        <v>334</v>
-      </c>
-      <c r="N69" t="s" s="2">
-        <v>335</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="M69" s="2"/>
+      <c r="N69" s="2"/>
       <c r="O69" t="s" s="2">
         <v>76</v>
       </c>
@@ -9651,13 +9662,13 @@
         <v>76</v>
       </c>
       <c r="W69" t="s" s="2">
-        <v>76</v>
+        <v>221</v>
       </c>
       <c r="X69" t="s" s="2">
-        <v>76</v>
+        <v>328</v>
       </c>
       <c r="Y69" t="s" s="2">
-        <v>76</v>
+        <v>329</v>
       </c>
       <c r="Z69" t="s" s="2">
         <v>76</v>
@@ -9675,7 +9686,7 @@
         <v>76</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>77</v>
@@ -9684,27 +9695,27 @@
         <v>85</v>
       </c>
       <c r="AH69" t="s" s="2">
-        <v>76</v>
+        <v>331</v>
       </c>
       <c r="AI69" t="s" s="2">
         <v>97</v>
       </c>
       <c r="AJ69" t="s" s="2">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="AK69" t="s" s="2">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="AL69" t="s" s="2">
-        <v>250</v>
+        <v>334</v>
       </c>
       <c r="AM69" t="s" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="70" hidden="true">
+    <row r="70">
       <c r="A70" t="s" s="2">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -9718,28 +9729,28 @@
         <v>85</v>
       </c>
       <c r="G70" t="s" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="H70" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="I70" t="s" s="2">
         <v>86</v>
       </c>
       <c r="J70" t="s" s="2">
-        <v>161</v>
+        <v>87</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="M70" t="s" s="2">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="N70" t="s" s="2">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="O70" t="s" s="2">
         <v>76</v>
@@ -9764,13 +9775,13 @@
         <v>76</v>
       </c>
       <c r="W70" t="s" s="2">
-        <v>217</v>
+        <v>76</v>
       </c>
       <c r="X70" t="s" s="2">
-        <v>344</v>
+        <v>76</v>
       </c>
       <c r="Y70" t="s" s="2">
-        <v>345</v>
+        <v>76</v>
       </c>
       <c r="Z70" t="s" s="2">
         <v>76</v>
@@ -9788,7 +9799,7 @@
         <v>76</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>77</v>
@@ -9803,13 +9814,13 @@
         <v>97</v>
       </c>
       <c r="AJ70" t="s" s="2">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="AK70" t="s" s="2">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="AL70" t="s" s="2">
-        <v>349</v>
+        <v>254</v>
       </c>
       <c r="AM70" t="s" s="2">
         <v>76</v>
@@ -9817,7 +9828,7 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -9834,24 +9845,26 @@
         <v>76</v>
       </c>
       <c r="H71" t="s" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="I71" t="s" s="2">
         <v>86</v>
       </c>
       <c r="J71" t="s" s="2">
-        <v>351</v>
+        <v>161</v>
       </c>
       <c r="K71" t="s" s="2">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="M71" t="s" s="2">
-        <v>354</v>
-      </c>
-      <c r="N71" s="2"/>
+        <v>346</v>
+      </c>
+      <c r="N71" t="s" s="2">
+        <v>347</v>
+      </c>
       <c r="O71" t="s" s="2">
         <v>76</v>
       </c>
@@ -9875,13 +9888,13 @@
         <v>76</v>
       </c>
       <c r="W71" t="s" s="2">
-        <v>76</v>
+        <v>221</v>
       </c>
       <c r="X71" t="s" s="2">
-        <v>76</v>
+        <v>348</v>
       </c>
       <c r="Y71" t="s" s="2">
-        <v>76</v>
+        <v>349</v>
       </c>
       <c r="Z71" t="s" s="2">
         <v>76</v>
@@ -9899,7 +9912,7 @@
         <v>76</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>77</v>
@@ -9914,13 +9927,13 @@
         <v>97</v>
       </c>
       <c r="AJ71" t="s" s="2">
-        <v>102</v>
+        <v>351</v>
       </c>
       <c r="AK71" t="s" s="2">
-        <v>102</v>
+        <v>352</v>
       </c>
       <c r="AL71" t="s" s="2">
-        <v>76</v>
+        <v>353</v>
       </c>
       <c r="AM71" t="s" s="2">
         <v>76</v>
@@ -9928,7 +9941,7 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -9951,15 +9964,17 @@
         <v>86</v>
       </c>
       <c r="J72" t="s" s="2">
-        <v>252</v>
+        <v>355</v>
       </c>
       <c r="K72" t="s" s="2">
+        <v>356</v>
+      </c>
+      <c r="L72" t="s" s="2">
         <v>357</v>
       </c>
-      <c r="L72" t="s" s="2">
+      <c r="M72" t="s" s="2">
         <v>358</v>
       </c>
-      <c r="M72" s="2"/>
       <c r="N72" s="2"/>
       <c r="O72" t="s" s="2">
         <v>76</v>
@@ -10023,13 +10038,13 @@
         <v>97</v>
       </c>
       <c r="AJ72" t="s" s="2">
-        <v>184</v>
+        <v>102</v>
       </c>
       <c r="AK72" t="s" s="2">
-        <v>360</v>
+        <v>102</v>
       </c>
       <c r="AL72" t="s" s="2">
-        <v>258</v>
+        <v>76</v>
       </c>
       <c r="AM72" t="s" s="2">
         <v>76</v>
@@ -10037,7 +10052,7 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
@@ -10057,21 +10072,19 @@
         <v>76</v>
       </c>
       <c r="I73" t="s" s="2">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="J73" t="s" s="2">
+        <v>256</v>
+      </c>
+      <c r="K73" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="L73" t="s" s="2">
         <v>362</v>
       </c>
-      <c r="K73" t="s" s="2">
-        <v>519</v>
-      </c>
-      <c r="L73" t="s" s="2">
-        <v>520</v>
-      </c>
       <c r="M73" s="2"/>
-      <c r="N73" t="s" s="2">
-        <v>521</v>
-      </c>
+      <c r="N73" s="2"/>
       <c r="O73" t="s" s="2">
         <v>76</v>
       </c>
@@ -10119,7 +10132,7 @@
         <v>76</v>
       </c>
       <c r="AE73" t="s" s="2">
-        <v>518</v>
+        <v>363</v>
       </c>
       <c r="AF73" t="s" s="2">
         <v>77</v>
@@ -10134,21 +10147,21 @@
         <v>97</v>
       </c>
       <c r="AJ73" t="s" s="2">
+        <v>184</v>
+      </c>
+      <c r="AK73" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="AL73" t="s" s="2">
+        <v>262</v>
+      </c>
+      <c r="AM73" t="s" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="74" hidden="true">
+      <c r="A74" t="s" s="2">
         <v>522</v>
-      </c>
-      <c r="AK73" t="s" s="2">
-        <v>523</v>
-      </c>
-      <c r="AL73" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AM73" t="s" s="2">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="s" s="2">
-        <v>524</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
@@ -10159,10 +10172,10 @@
         <v>77</v>
       </c>
       <c r="F74" t="s" s="2">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="G74" t="s" s="2">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="H74" t="s" s="2">
         <v>76</v>
@@ -10171,17 +10184,17 @@
         <v>76</v>
       </c>
       <c r="J74" t="s" s="2">
-        <v>525</v>
+        <v>366</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="M74" s="2"/>
       <c r="N74" t="s" s="2">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="O74" t="s" s="2">
         <v>76</v>
@@ -10230,13 +10243,13 @@
         <v>76</v>
       </c>
       <c r="AE74" t="s" s="2">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="AF74" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AG74" t="s" s="2">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="AH74" t="s" s="2">
         <v>76</v>
@@ -10245,20 +10258,131 @@
         <v>97</v>
       </c>
       <c r="AJ74" t="s" s="2">
-        <v>76</v>
+        <v>526</v>
       </c>
       <c r="AK74" t="s" s="2">
+        <v>527</v>
+      </c>
+      <c r="AL74" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AM74" t="s" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s" s="2">
+        <v>528</v>
+      </c>
+      <c r="B75" s="2"/>
+      <c r="C75" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="D75" s="2"/>
+      <c r="E75" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="F75" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G75" t="s" s="2">
+        <v>86</v>
+      </c>
+      <c r="H75" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="I75" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="J75" t="s" s="2">
+        <v>529</v>
+      </c>
+      <c r="K75" t="s" s="2">
+        <v>530</v>
+      </c>
+      <c r="L75" t="s" s="2">
+        <v>531</v>
+      </c>
+      <c r="M75" s="2"/>
+      <c r="N75" t="s" s="2">
+        <v>532</v>
+      </c>
+      <c r="O75" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="P75" s="2"/>
+      <c r="Q75" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="R75" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="S75" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="T75" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="U75" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="V75" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="W75" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="X75" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="Y75" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="Z75" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AA75" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AB75" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AC75" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AD75" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE75" t="s" s="2">
+        <v>528</v>
+      </c>
+      <c r="AF75" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AG75" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH75" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AI75" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="AJ75" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AK75" t="s" s="2">
         <v>102</v>
       </c>
-      <c r="AL74" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AM74" t="s" s="2">
+      <c r="AL75" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AM75" t="s" s="2">
         <v>76</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AM74">
+  <autoFilter ref="A1:AM75">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -10268,7 +10392,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI73">
+  <conditionalFormatting sqref="A2:AI74">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>